<commit_message>
add tag for block
</commit_message>
<xml_diff>
--- a/_Out/Server/NFDataCfg/Excel_Ini/Block.xlsx
+++ b/_Out/Server/NFDataCfg/Excel_Ini/Block.xlsx
@@ -27,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="13" uniqueCount="13">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="14" uniqueCount="14">
   <si>
     <t>ID</t>
     <phoneticPr fontId="1" type="noConversion"/>
@@ -78,6 +78,10 @@
   </si>
   <si>
     <t>DownID</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Tag</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
 </sst>
@@ -135,7 +139,10 @@
   <cellStyles count="1">
     <cellStyle name="常规" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="3">
+  <dxfs count="4">
+    <dxf>
+      <numFmt numFmtId="30" formatCode="@"/>
+    </dxf>
     <dxf>
       <numFmt numFmtId="30" formatCode="@"/>
     </dxf>
@@ -191,13 +198,14 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="1" name="表1" displayName="表1" ref="A1:M53" tableType="xml" totalsRowShown="0" connectionId="1">
-  <autoFilter ref="A1:M53"/>
-  <tableColumns count="13">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="1" name="表1" displayName="表1" ref="A1:N53" tableType="xml" totalsRowShown="0" connectionId="1">
+  <autoFilter ref="A1:N53"/>
+  <tableColumns count="14">
     <tableColumn id="1" uniqueName="ID" name="ID">
       <xmlColumnPr mapId="1" xpath="/XML/Object/@ID" xmlDataType="string"/>
     </tableColumn>
-    <tableColumn id="2" uniqueName="TaskName" name="LeftSide" dataDxfId="2">
+    <tableColumn id="14" uniqueName="14" name="Tag" dataDxfId="0"/>
+    <tableColumn id="2" uniqueName="TaskName" name="LeftSide" dataDxfId="3">
       <xmlColumnPr mapId="1" xpath="/XML/Object/@TaskName" xmlDataType="string"/>
     </tableColumn>
     <tableColumn id="3" uniqueName="Type" name="RightSide">
@@ -224,8 +232,8 @@
     <tableColumn id="10" uniqueName="AwardPack" name="LeftID">
       <xmlColumnPr mapId="1" xpath="/XML/Object/@AwardPack" xmlDataType="string"/>
     </tableColumn>
-    <tableColumn id="11" uniqueName="11" name="RightID" dataDxfId="1"/>
-    <tableColumn id="12" uniqueName="12" name="TopID" dataDxfId="0"/>
+    <tableColumn id="11" uniqueName="11" name="RightID" dataDxfId="2"/>
+    <tableColumn id="12" uniqueName="12" name="TopID" dataDxfId="1"/>
     <tableColumn id="13" uniqueName="13" name="DownID"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
@@ -495,431 +503,486 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:M53"/>
+  <dimension ref="A1:N53"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="H10" sqref="H10"/>
+      <selection activeCell="B2" sqref="B2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.5" x14ac:dyDescent="0.15"/>
   <cols>
-    <col min="1" max="1" width="17.375" customWidth="1"/>
-    <col min="2" max="2" width="12.75" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="14" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="15.25" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="21.5" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="14" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="24.625" customWidth="1"/>
-    <col min="8" max="8" width="27" customWidth="1"/>
-    <col min="9" max="13" width="14" bestFit="1" customWidth="1"/>
+    <col min="1" max="2" width="17.375" customWidth="1"/>
+    <col min="3" max="3" width="12.75" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="14" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="15.25" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="21.5" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="14" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="24.625" customWidth="1"/>
+    <col min="9" max="9" width="27" customWidth="1"/>
+    <col min="10" max="14" width="14" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:13" x14ac:dyDescent="0.15">
+    <row r="1" spans="1:14" x14ac:dyDescent="0.15">
       <c r="A1" t="s">
         <v>0</v>
       </c>
       <c r="B1" t="s">
+        <v>13</v>
+      </c>
+      <c r="C1" t="s">
         <v>1</v>
       </c>
-      <c r="C1" t="s">
+      <c r="D1" t="s">
         <v>2</v>
       </c>
-      <c r="D1" t="s">
+      <c r="E1" t="s">
         <v>3</v>
       </c>
-      <c r="E1" t="s">
+      <c r="F1" t="s">
         <v>4</v>
       </c>
-      <c r="F1" t="s">
+      <c r="G1" t="s">
         <v>5</v>
       </c>
-      <c r="G1" t="s">
+      <c r="H1" t="s">
         <v>6</v>
       </c>
-      <c r="H1" t="s">
+      <c r="I1" t="s">
         <v>7</v>
       </c>
-      <c r="I1" t="s">
+      <c r="J1" t="s">
         <v>8</v>
       </c>
-      <c r="J1" t="s">
+      <c r="K1" t="s">
         <v>9</v>
       </c>
-      <c r="K1" t="s">
+      <c r="L1" t="s">
         <v>10</v>
       </c>
-      <c r="L1" t="s">
+      <c r="M1" t="s">
         <v>11</v>
       </c>
-      <c r="M1" t="s">
+      <c r="N1" t="s">
         <v>12</v>
       </c>
     </row>
-    <row r="2" spans="1:13" x14ac:dyDescent="0.15">
+    <row r="2" spans="1:14" x14ac:dyDescent="0.15">
       <c r="A2" s="1"/>
       <c r="B2" s="1"/>
-      <c r="D2" s="1"/>
+      <c r="C2" s="1"/>
       <c r="E2" s="1"/>
-      <c r="J2" s="1"/>
+      <c r="F2" s="1"/>
       <c r="K2" s="1"/>
       <c r="L2" s="1"/>
-    </row>
-    <row r="3" spans="1:13" x14ac:dyDescent="0.15">
+      <c r="M2" s="1"/>
+    </row>
+    <row r="3" spans="1:14" x14ac:dyDescent="0.15">
       <c r="A3" s="1"/>
       <c r="B3" s="1"/>
-      <c r="D3" s="1"/>
+      <c r="C3" s="1"/>
       <c r="E3" s="1"/>
-      <c r="J3" s="1"/>
+      <c r="F3" s="1"/>
       <c r="K3" s="1"/>
       <c r="L3" s="1"/>
-    </row>
-    <row r="4" spans="1:13" x14ac:dyDescent="0.15">
+      <c r="M3" s="1"/>
+    </row>
+    <row r="4" spans="1:14" x14ac:dyDescent="0.15">
       <c r="A4" s="1"/>
-    </row>
-    <row r="5" spans="1:13" x14ac:dyDescent="0.15">
+      <c r="B4" s="1"/>
+    </row>
+    <row r="5" spans="1:14" x14ac:dyDescent="0.15">
       <c r="A5" s="1"/>
       <c r="B5" s="1"/>
-      <c r="D5" s="1"/>
+      <c r="C5" s="1"/>
       <c r="E5" s="1"/>
-      <c r="J5" s="1"/>
+      <c r="F5" s="1"/>
       <c r="K5" s="1"/>
       <c r="L5" s="1"/>
-    </row>
-    <row r="6" spans="1:13" x14ac:dyDescent="0.15">
+      <c r="M5" s="1"/>
+    </row>
+    <row r="6" spans="1:14" x14ac:dyDescent="0.15">
       <c r="A6" s="1"/>
       <c r="B6" s="1"/>
-      <c r="D6" s="1"/>
+      <c r="C6" s="1"/>
       <c r="E6" s="1"/>
-      <c r="J6" s="1"/>
+      <c r="F6" s="1"/>
       <c r="K6" s="1"/>
       <c r="L6" s="1"/>
-    </row>
-    <row r="7" spans="1:13" x14ac:dyDescent="0.15">
+      <c r="M6" s="1"/>
+    </row>
+    <row r="7" spans="1:14" x14ac:dyDescent="0.15">
       <c r="A7" s="1"/>
-    </row>
-    <row r="8" spans="1:13" x14ac:dyDescent="0.15">
+      <c r="B7" s="1"/>
+    </row>
+    <row r="8" spans="1:14" x14ac:dyDescent="0.15">
       <c r="A8" s="1"/>
       <c r="B8" s="1"/>
-      <c r="D8" s="1"/>
+      <c r="C8" s="1"/>
       <c r="E8" s="1"/>
-      <c r="J8" s="1"/>
+      <c r="F8" s="1"/>
       <c r="K8" s="1"/>
       <c r="L8" s="1"/>
-    </row>
-    <row r="9" spans="1:13" x14ac:dyDescent="0.15">
+      <c r="M8" s="1"/>
+    </row>
+    <row r="9" spans="1:14" x14ac:dyDescent="0.15">
       <c r="A9" s="1"/>
       <c r="B9" s="1"/>
-      <c r="D9" s="1"/>
+      <c r="C9" s="1"/>
       <c r="E9" s="1"/>
-      <c r="J9" s="1"/>
+      <c r="F9" s="1"/>
       <c r="K9" s="1"/>
       <c r="L9" s="1"/>
-    </row>
-    <row r="10" spans="1:13" x14ac:dyDescent="0.15">
+      <c r="M9" s="1"/>
+    </row>
+    <row r="10" spans="1:14" x14ac:dyDescent="0.15">
       <c r="A10" s="1"/>
-    </row>
-    <row r="11" spans="1:13" x14ac:dyDescent="0.15">
+      <c r="B10" s="1"/>
+    </row>
+    <row r="11" spans="1:14" x14ac:dyDescent="0.15">
       <c r="A11" s="1"/>
       <c r="B11" s="1"/>
-      <c r="D11" s="1"/>
+      <c r="C11" s="1"/>
       <c r="E11" s="1"/>
-      <c r="J11" s="1"/>
+      <c r="F11" s="1"/>
       <c r="K11" s="1"/>
       <c r="L11" s="1"/>
-    </row>
-    <row r="12" spans="1:13" x14ac:dyDescent="0.15">
+      <c r="M11" s="1"/>
+    </row>
+    <row r="12" spans="1:14" x14ac:dyDescent="0.15">
       <c r="A12" s="1"/>
       <c r="B12" s="1"/>
-      <c r="D12" s="1"/>
+      <c r="C12" s="1"/>
       <c r="E12" s="1"/>
-      <c r="J12" s="1"/>
+      <c r="F12" s="1"/>
       <c r="K12" s="1"/>
       <c r="L12" s="1"/>
-    </row>
-    <row r="13" spans="1:13" x14ac:dyDescent="0.15">
+      <c r="M12" s="1"/>
+    </row>
+    <row r="13" spans="1:14" x14ac:dyDescent="0.15">
       <c r="A13" s="1"/>
-    </row>
-    <row r="14" spans="1:13" x14ac:dyDescent="0.15">
+      <c r="B13" s="1"/>
+    </row>
+    <row r="14" spans="1:14" x14ac:dyDescent="0.15">
       <c r="A14" s="1"/>
       <c r="B14" s="1"/>
-      <c r="D14" s="1"/>
+      <c r="C14" s="1"/>
       <c r="E14" s="1"/>
-      <c r="J14" s="1"/>
+      <c r="F14" s="1"/>
       <c r="K14" s="1"/>
       <c r="L14" s="1"/>
-    </row>
-    <row r="15" spans="1:13" x14ac:dyDescent="0.15">
+      <c r="M14" s="1"/>
+    </row>
+    <row r="15" spans="1:14" x14ac:dyDescent="0.15">
       <c r="A15" s="1"/>
       <c r="B15" s="1"/>
-      <c r="D15" s="1"/>
+      <c r="C15" s="1"/>
       <c r="E15" s="1"/>
-      <c r="J15" s="1"/>
+      <c r="F15" s="1"/>
       <c r="K15" s="1"/>
       <c r="L15" s="1"/>
-    </row>
-    <row r="16" spans="1:13" x14ac:dyDescent="0.15">
+      <c r="M15" s="1"/>
+    </row>
+    <row r="16" spans="1:14" x14ac:dyDescent="0.15">
       <c r="A16" s="1"/>
-    </row>
-    <row r="17" spans="1:12" x14ac:dyDescent="0.15">
+      <c r="B16" s="1"/>
+    </row>
+    <row r="17" spans="1:13" x14ac:dyDescent="0.15">
       <c r="A17" s="1"/>
       <c r="B17" s="1"/>
-      <c r="D17" s="1"/>
+      <c r="C17" s="1"/>
       <c r="E17" s="1"/>
-      <c r="J17" s="1"/>
+      <c r="F17" s="1"/>
       <c r="K17" s="1"/>
       <c r="L17" s="1"/>
-    </row>
-    <row r="18" spans="1:12" x14ac:dyDescent="0.15">
+      <c r="M17" s="1"/>
+    </row>
+    <row r="18" spans="1:13" x14ac:dyDescent="0.15">
       <c r="A18" s="1"/>
       <c r="B18" s="1"/>
-      <c r="D18" s="1"/>
+      <c r="C18" s="1"/>
       <c r="E18" s="1"/>
-      <c r="J18" s="1"/>
+      <c r="F18" s="1"/>
       <c r="K18" s="1"/>
       <c r="L18" s="1"/>
-    </row>
-    <row r="19" spans="1:12" x14ac:dyDescent="0.15">
+      <c r="M18" s="1"/>
+    </row>
+    <row r="19" spans="1:13" x14ac:dyDescent="0.15">
       <c r="A19" s="1"/>
-    </row>
-    <row r="20" spans="1:12" x14ac:dyDescent="0.15">
+      <c r="B19" s="1"/>
+    </row>
+    <row r="20" spans="1:13" x14ac:dyDescent="0.15">
       <c r="A20" s="1"/>
       <c r="B20" s="1"/>
-      <c r="D20" s="1"/>
+      <c r="C20" s="1"/>
       <c r="E20" s="1"/>
-      <c r="J20" s="1"/>
+      <c r="F20" s="1"/>
       <c r="K20" s="1"/>
       <c r="L20" s="1"/>
-    </row>
-    <row r="21" spans="1:12" x14ac:dyDescent="0.15">
+      <c r="M20" s="1"/>
+    </row>
+    <row r="21" spans="1:13" x14ac:dyDescent="0.15">
       <c r="A21" s="1"/>
       <c r="B21" s="1"/>
-      <c r="D21" s="1"/>
+      <c r="C21" s="1"/>
       <c r="E21" s="1"/>
-      <c r="J21" s="1"/>
+      <c r="F21" s="1"/>
       <c r="K21" s="1"/>
       <c r="L21" s="1"/>
-    </row>
-    <row r="22" spans="1:12" x14ac:dyDescent="0.15">
+      <c r="M21" s="1"/>
+    </row>
+    <row r="22" spans="1:13" x14ac:dyDescent="0.15">
       <c r="A22" s="1"/>
-    </row>
-    <row r="23" spans="1:12" x14ac:dyDescent="0.15">
+      <c r="B22" s="1"/>
+    </row>
+    <row r="23" spans="1:13" x14ac:dyDescent="0.15">
       <c r="A23" s="1"/>
       <c r="B23" s="1"/>
-      <c r="D23" s="1"/>
+      <c r="C23" s="1"/>
       <c r="E23" s="1"/>
-      <c r="J23" s="1"/>
+      <c r="F23" s="1"/>
       <c r="K23" s="1"/>
       <c r="L23" s="1"/>
-    </row>
-    <row r="24" spans="1:12" x14ac:dyDescent="0.15">
+      <c r="M23" s="1"/>
+    </row>
+    <row r="24" spans="1:13" x14ac:dyDescent="0.15">
       <c r="A24" s="1"/>
       <c r="B24" s="1"/>
-      <c r="D24" s="1"/>
+      <c r="C24" s="1"/>
       <c r="E24" s="1"/>
-      <c r="J24" s="1"/>
+      <c r="F24" s="1"/>
       <c r="K24" s="1"/>
       <c r="L24" s="1"/>
-    </row>
-    <row r="25" spans="1:12" x14ac:dyDescent="0.15">
+      <c r="M24" s="1"/>
+    </row>
+    <row r="25" spans="1:13" x14ac:dyDescent="0.15">
       <c r="A25" s="1"/>
-    </row>
-    <row r="26" spans="1:12" x14ac:dyDescent="0.15">
+      <c r="B25" s="1"/>
+    </row>
+    <row r="26" spans="1:13" x14ac:dyDescent="0.15">
       <c r="A26" s="1"/>
       <c r="B26" s="1"/>
-      <c r="D26" s="1"/>
+      <c r="C26" s="1"/>
       <c r="E26" s="1"/>
-      <c r="J26" s="1"/>
+      <c r="F26" s="1"/>
       <c r="K26" s="1"/>
       <c r="L26" s="1"/>
-    </row>
-    <row r="27" spans="1:12" x14ac:dyDescent="0.15">
+      <c r="M26" s="1"/>
+    </row>
+    <row r="27" spans="1:13" x14ac:dyDescent="0.15">
       <c r="A27" s="1"/>
       <c r="B27" s="1"/>
-      <c r="D27" s="1"/>
+      <c r="C27" s="1"/>
       <c r="E27" s="1"/>
-      <c r="J27" s="1"/>
+      <c r="F27" s="1"/>
       <c r="K27" s="1"/>
       <c r="L27" s="1"/>
-    </row>
-    <row r="28" spans="1:12" x14ac:dyDescent="0.15">
+      <c r="M27" s="1"/>
+    </row>
+    <row r="28" spans="1:13" x14ac:dyDescent="0.15">
       <c r="A28" s="1"/>
-    </row>
-    <row r="29" spans="1:12" x14ac:dyDescent="0.15">
+      <c r="B28" s="1"/>
+    </row>
+    <row r="29" spans="1:13" x14ac:dyDescent="0.15">
       <c r="A29" s="1"/>
       <c r="B29" s="1"/>
-      <c r="D29" s="1"/>
+      <c r="C29" s="1"/>
       <c r="E29" s="1"/>
-      <c r="J29" s="1"/>
+      <c r="F29" s="1"/>
       <c r="K29" s="1"/>
       <c r="L29" s="1"/>
-    </row>
-    <row r="30" spans="1:12" x14ac:dyDescent="0.15">
+      <c r="M29" s="1"/>
+    </row>
+    <row r="30" spans="1:13" x14ac:dyDescent="0.15">
       <c r="A30" s="1"/>
       <c r="B30" s="1"/>
-      <c r="D30" s="1"/>
+      <c r="C30" s="1"/>
       <c r="E30" s="1"/>
-      <c r="J30" s="1"/>
+      <c r="F30" s="1"/>
       <c r="K30" s="1"/>
       <c r="L30" s="1"/>
-    </row>
-    <row r="31" spans="1:12" x14ac:dyDescent="0.15">
+      <c r="M30" s="1"/>
+    </row>
+    <row r="31" spans="1:13" x14ac:dyDescent="0.15">
       <c r="A31" s="1"/>
-    </row>
-    <row r="32" spans="1:12" x14ac:dyDescent="0.15">
+      <c r="B31" s="1"/>
+    </row>
+    <row r="32" spans="1:13" x14ac:dyDescent="0.15">
       <c r="A32" s="1"/>
       <c r="B32" s="1"/>
-      <c r="D32" s="1"/>
+      <c r="C32" s="1"/>
       <c r="E32" s="1"/>
-      <c r="J32" s="1"/>
+      <c r="F32" s="1"/>
       <c r="K32" s="1"/>
       <c r="L32" s="1"/>
-    </row>
-    <row r="33" spans="1:12" x14ac:dyDescent="0.15">
+      <c r="M32" s="1"/>
+    </row>
+    <row r="33" spans="1:13" x14ac:dyDescent="0.15">
       <c r="A33" s="1"/>
       <c r="B33" s="1"/>
-      <c r="D33" s="1"/>
+      <c r="C33" s="1"/>
       <c r="E33" s="1"/>
-      <c r="J33" s="1"/>
+      <c r="F33" s="1"/>
       <c r="K33" s="1"/>
       <c r="L33" s="1"/>
-    </row>
-    <row r="34" spans="1:12" x14ac:dyDescent="0.15">
+      <c r="M33" s="1"/>
+    </row>
+    <row r="34" spans="1:13" x14ac:dyDescent="0.15">
       <c r="A34" s="1"/>
-    </row>
-    <row r="35" spans="1:12" x14ac:dyDescent="0.15">
+      <c r="B34" s="1"/>
+    </row>
+    <row r="35" spans="1:13" x14ac:dyDescent="0.15">
       <c r="A35" s="1"/>
       <c r="B35" s="1"/>
-      <c r="D35" s="1"/>
+      <c r="C35" s="1"/>
       <c r="E35" s="1"/>
-      <c r="J35" s="1"/>
+      <c r="F35" s="1"/>
       <c r="K35" s="1"/>
       <c r="L35" s="1"/>
-    </row>
-    <row r="36" spans="1:12" x14ac:dyDescent="0.15">
+      <c r="M35" s="1"/>
+    </row>
+    <row r="36" spans="1:13" x14ac:dyDescent="0.15">
       <c r="A36" s="1"/>
       <c r="B36" s="1"/>
-      <c r="D36" s="1"/>
+      <c r="C36" s="1"/>
       <c r="E36" s="1"/>
-      <c r="J36" s="1"/>
+      <c r="F36" s="1"/>
       <c r="K36" s="1"/>
       <c r="L36" s="1"/>
-    </row>
-    <row r="37" spans="1:12" x14ac:dyDescent="0.15">
+      <c r="M36" s="1"/>
+    </row>
+    <row r="37" spans="1:13" x14ac:dyDescent="0.15">
       <c r="A37" s="1"/>
-    </row>
-    <row r="38" spans="1:12" x14ac:dyDescent="0.15">
+      <c r="B37" s="1"/>
+    </row>
+    <row r="38" spans="1:13" x14ac:dyDescent="0.15">
       <c r="A38" s="1"/>
       <c r="B38" s="1"/>
-      <c r="D38" s="1"/>
+      <c r="C38" s="1"/>
       <c r="E38" s="1"/>
-      <c r="J38" s="1"/>
+      <c r="F38" s="1"/>
       <c r="K38" s="1"/>
       <c r="L38" s="1"/>
-    </row>
-    <row r="39" spans="1:12" x14ac:dyDescent="0.15">
+      <c r="M38" s="1"/>
+    </row>
+    <row r="39" spans="1:13" x14ac:dyDescent="0.15">
       <c r="A39" s="1"/>
       <c r="B39" s="1"/>
-      <c r="D39" s="1"/>
+      <c r="C39" s="1"/>
       <c r="E39" s="1"/>
-      <c r="J39" s="1"/>
+      <c r="F39" s="1"/>
       <c r="K39" s="1"/>
       <c r="L39" s="1"/>
-    </row>
-    <row r="40" spans="1:12" x14ac:dyDescent="0.15">
+      <c r="M39" s="1"/>
+    </row>
+    <row r="40" spans="1:13" x14ac:dyDescent="0.15">
       <c r="A40" s="1"/>
-    </row>
-    <row r="41" spans="1:12" x14ac:dyDescent="0.15">
+      <c r="B40" s="1"/>
+    </row>
+    <row r="41" spans="1:13" x14ac:dyDescent="0.15">
       <c r="A41" s="1"/>
       <c r="B41" s="1"/>
-      <c r="D41" s="1"/>
+      <c r="C41" s="1"/>
       <c r="E41" s="1"/>
-      <c r="J41" s="1"/>
+      <c r="F41" s="1"/>
       <c r="K41" s="1"/>
       <c r="L41" s="1"/>
-    </row>
-    <row r="42" spans="1:12" x14ac:dyDescent="0.15">
+      <c r="M41" s="1"/>
+    </row>
+    <row r="42" spans="1:13" x14ac:dyDescent="0.15">
       <c r="A42" s="1"/>
       <c r="B42" s="1"/>
-      <c r="D42" s="1"/>
+      <c r="C42" s="1"/>
       <c r="E42" s="1"/>
-      <c r="J42" s="1"/>
+      <c r="F42" s="1"/>
       <c r="K42" s="1"/>
       <c r="L42" s="1"/>
-    </row>
-    <row r="43" spans="1:12" x14ac:dyDescent="0.15">
+      <c r="M42" s="1"/>
+    </row>
+    <row r="43" spans="1:13" x14ac:dyDescent="0.15">
       <c r="A43" s="1"/>
-    </row>
-    <row r="44" spans="1:12" x14ac:dyDescent="0.15">
+      <c r="B43" s="1"/>
+    </row>
+    <row r="44" spans="1:13" x14ac:dyDescent="0.15">
       <c r="A44" s="1"/>
       <c r="B44" s="1"/>
-      <c r="D44" s="1"/>
+      <c r="C44" s="1"/>
       <c r="E44" s="1"/>
-      <c r="J44" s="1"/>
+      <c r="F44" s="1"/>
       <c r="K44" s="1"/>
       <c r="L44" s="1"/>
-    </row>
-    <row r="45" spans="1:12" x14ac:dyDescent="0.15">
+      <c r="M44" s="1"/>
+    </row>
+    <row r="45" spans="1:13" x14ac:dyDescent="0.15">
       <c r="A45" s="1"/>
       <c r="B45" s="1"/>
-      <c r="D45" s="1"/>
+      <c r="C45" s="1"/>
       <c r="E45" s="1"/>
-      <c r="J45" s="1"/>
+      <c r="F45" s="1"/>
       <c r="K45" s="1"/>
       <c r="L45" s="1"/>
-    </row>
-    <row r="46" spans="1:12" x14ac:dyDescent="0.15">
+      <c r="M45" s="1"/>
+    </row>
+    <row r="46" spans="1:13" x14ac:dyDescent="0.15">
       <c r="A46" s="1"/>
-    </row>
-    <row r="47" spans="1:12" x14ac:dyDescent="0.15">
+      <c r="B46" s="1"/>
+    </row>
+    <row r="47" spans="1:13" x14ac:dyDescent="0.15">
       <c r="A47" s="1"/>
       <c r="B47" s="1"/>
-      <c r="D47" s="1"/>
+      <c r="C47" s="1"/>
       <c r="E47" s="1"/>
-      <c r="J47" s="1"/>
+      <c r="F47" s="1"/>
       <c r="K47" s="1"/>
       <c r="L47" s="1"/>
-    </row>
-    <row r="48" spans="1:12" x14ac:dyDescent="0.15">
+      <c r="M47" s="1"/>
+    </row>
+    <row r="48" spans="1:13" x14ac:dyDescent="0.15">
       <c r="A48" s="1"/>
       <c r="B48" s="1"/>
-      <c r="D48" s="1"/>
+      <c r="C48" s="1"/>
       <c r="E48" s="1"/>
-      <c r="J48" s="1"/>
+      <c r="F48" s="1"/>
       <c r="K48" s="1"/>
       <c r="L48" s="1"/>
-    </row>
-    <row r="49" spans="1:12" x14ac:dyDescent="0.15">
+      <c r="M48" s="1"/>
+    </row>
+    <row r="49" spans="1:13" x14ac:dyDescent="0.15">
       <c r="A49" s="1"/>
-    </row>
-    <row r="50" spans="1:12" x14ac:dyDescent="0.15">
+      <c r="B49" s="1"/>
+    </row>
+    <row r="50" spans="1:13" x14ac:dyDescent="0.15">
       <c r="A50" s="1"/>
       <c r="B50" s="1"/>
-      <c r="D50" s="1"/>
+      <c r="C50" s="1"/>
       <c r="E50" s="1"/>
-      <c r="J50" s="1"/>
+      <c r="F50" s="1"/>
       <c r="K50" s="1"/>
       <c r="L50" s="1"/>
-    </row>
-    <row r="51" spans="1:12" x14ac:dyDescent="0.15">
+      <c r="M50" s="1"/>
+    </row>
+    <row r="51" spans="1:13" x14ac:dyDescent="0.15">
       <c r="A51" s="1"/>
       <c r="B51" s="1"/>
-      <c r="D51" s="1"/>
+      <c r="C51" s="1"/>
       <c r="E51" s="1"/>
-      <c r="J51" s="1"/>
+      <c r="F51" s="1"/>
       <c r="K51" s="1"/>
       <c r="L51" s="1"/>
-    </row>
-    <row r="52" spans="1:12" x14ac:dyDescent="0.15">
+      <c r="M51" s="1"/>
+    </row>
+    <row r="52" spans="1:13" x14ac:dyDescent="0.15">
       <c r="A52" s="1"/>
-    </row>
-    <row r="53" spans="1:12" x14ac:dyDescent="0.15">
+      <c r="B52" s="1"/>
+    </row>
+    <row r="53" spans="1:13" x14ac:dyDescent="0.15">
       <c r="A53" s="1"/>
       <c r="B53" s="1"/>
-      <c r="D53" s="1"/>
+      <c r="C53" s="1"/>
       <c r="E53" s="1"/>
-      <c r="J53" s="1"/>
+      <c r="F53" s="1"/>
       <c r="K53" s="1"/>
       <c r="L53" s="1"/>
+      <c r="M53" s="1"/>
     </row>
   </sheetData>
   <phoneticPr fontId="1" type="noConversion"/>

</xml_diff>

<commit_message>
remove unused property for block
</commit_message>
<xml_diff>
--- a/_Out/Server/NFDataCfg/Excel_Ini/Block.xlsx
+++ b/_Out/Server/NFDataCfg/Excel_Ini/Block.xlsx
@@ -27,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="14" uniqueCount="14">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="10" uniqueCount="10">
   <si>
     <t>ID</t>
     <phoneticPr fontId="1" type="noConversion"/>
@@ -62,22 +62,6 @@
   </si>
   <si>
     <t>RightDownSide</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>LeftID</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>RightID</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>TopID</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>DownID</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
@@ -139,13 +123,7 @@
   <cellStyles count="1">
     <cellStyle name="常规" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="4">
-    <dxf>
-      <numFmt numFmtId="30" formatCode="@"/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="30" formatCode="@"/>
-    </dxf>
+  <dxfs count="2">
     <dxf>
       <numFmt numFmtId="30" formatCode="@"/>
     </dxf>
@@ -198,14 +176,14 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="1" name="表1" displayName="表1" ref="A1:N53" tableType="xml" totalsRowShown="0" connectionId="1">
-  <autoFilter ref="A1:N53"/>
-  <tableColumns count="14">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="1" name="表1" displayName="表1" ref="A1:J53" tableType="xml" totalsRowShown="0" connectionId="1">
+  <autoFilter ref="A1:J53"/>
+  <tableColumns count="10">
     <tableColumn id="1" uniqueName="ID" name="ID">
       <xmlColumnPr mapId="1" xpath="/XML/Object/@ID" xmlDataType="string"/>
     </tableColumn>
-    <tableColumn id="14" uniqueName="14" name="Tag" dataDxfId="0"/>
-    <tableColumn id="2" uniqueName="TaskName" name="LeftSide" dataDxfId="3">
+    <tableColumn id="14" uniqueName="14" name="Tag" dataDxfId="1"/>
+    <tableColumn id="2" uniqueName="TaskName" name="LeftSide" dataDxfId="0">
       <xmlColumnPr mapId="1" xpath="/XML/Object/@TaskName" xmlDataType="string"/>
     </tableColumn>
     <tableColumn id="3" uniqueName="Type" name="RightSide">
@@ -229,12 +207,6 @@
     <tableColumn id="9" uniqueName="AwardGold" name="RightDownSide">
       <xmlColumnPr mapId="1" xpath="/XML/Object/@AwardGold" xmlDataType="integer"/>
     </tableColumn>
-    <tableColumn id="10" uniqueName="AwardPack" name="LeftID">
-      <xmlColumnPr mapId="1" xpath="/XML/Object/@AwardPack" xmlDataType="string"/>
-    </tableColumn>
-    <tableColumn id="11" uniqueName="11" name="RightID" dataDxfId="2"/>
-    <tableColumn id="12" uniqueName="12" name="TopID" dataDxfId="1"/>
-    <tableColumn id="13" uniqueName="13" name="DownID"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -503,10 +475,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:N53"/>
+  <dimension ref="A1:J53"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B2" sqref="B2"/>
+    <sheetView tabSelected="1" topLeftCell="B1" workbookViewId="0">
+      <selection activeCell="K1" sqref="K1:K1048576"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.5" x14ac:dyDescent="0.15"/>
@@ -519,15 +491,15 @@
     <col min="7" max="7" width="14" bestFit="1" customWidth="1"/>
     <col min="8" max="8" width="24.625" customWidth="1"/>
     <col min="9" max="9" width="27" customWidth="1"/>
-    <col min="10" max="14" width="14" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="14" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:14" x14ac:dyDescent="0.15">
+    <row r="1" spans="1:10" x14ac:dyDescent="0.15">
       <c r="A1" t="s">
         <v>0</v>
       </c>
       <c r="B1" t="s">
-        <v>13</v>
+        <v>9</v>
       </c>
       <c r="C1" t="s">
         <v>1</v>
@@ -553,436 +525,319 @@
       <c r="J1" t="s">
         <v>8</v>
       </c>
-      <c r="K1" t="s">
-        <v>9</v>
-      </c>
-      <c r="L1" t="s">
-        <v>10</v>
-      </c>
-      <c r="M1" t="s">
-        <v>11</v>
-      </c>
-      <c r="N1" t="s">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="2" spans="1:14" x14ac:dyDescent="0.15">
+    </row>
+    <row r="2" spans="1:10" x14ac:dyDescent="0.15">
       <c r="A2" s="1"/>
       <c r="B2" s="1"/>
       <c r="C2" s="1"/>
       <c r="E2" s="1"/>
       <c r="F2" s="1"/>
-      <c r="K2" s="1"/>
-      <c r="L2" s="1"/>
-      <c r="M2" s="1"/>
-    </row>
-    <row r="3" spans="1:14" x14ac:dyDescent="0.15">
+    </row>
+    <row r="3" spans="1:10" x14ac:dyDescent="0.15">
       <c r="A3" s="1"/>
       <c r="B3" s="1"/>
       <c r="C3" s="1"/>
       <c r="E3" s="1"/>
       <c r="F3" s="1"/>
-      <c r="K3" s="1"/>
-      <c r="L3" s="1"/>
-      <c r="M3" s="1"/>
-    </row>
-    <row r="4" spans="1:14" x14ac:dyDescent="0.15">
+    </row>
+    <row r="4" spans="1:10" x14ac:dyDescent="0.15">
       <c r="A4" s="1"/>
       <c r="B4" s="1"/>
     </row>
-    <row r="5" spans="1:14" x14ac:dyDescent="0.15">
+    <row r="5" spans="1:10" x14ac:dyDescent="0.15">
       <c r="A5" s="1"/>
       <c r="B5" s="1"/>
       <c r="C5" s="1"/>
       <c r="E5" s="1"/>
       <c r="F5" s="1"/>
-      <c r="K5" s="1"/>
-      <c r="L5" s="1"/>
-      <c r="M5" s="1"/>
-    </row>
-    <row r="6" spans="1:14" x14ac:dyDescent="0.15">
+    </row>
+    <row r="6" spans="1:10" x14ac:dyDescent="0.15">
       <c r="A6" s="1"/>
       <c r="B6" s="1"/>
       <c r="C6" s="1"/>
       <c r="E6" s="1"/>
       <c r="F6" s="1"/>
-      <c r="K6" s="1"/>
-      <c r="L6" s="1"/>
-      <c r="M6" s="1"/>
-    </row>
-    <row r="7" spans="1:14" x14ac:dyDescent="0.15">
+    </row>
+    <row r="7" spans="1:10" x14ac:dyDescent="0.15">
       <c r="A7" s="1"/>
       <c r="B7" s="1"/>
     </row>
-    <row r="8" spans="1:14" x14ac:dyDescent="0.15">
+    <row r="8" spans="1:10" x14ac:dyDescent="0.15">
       <c r="A8" s="1"/>
       <c r="B8" s="1"/>
       <c r="C8" s="1"/>
       <c r="E8" s="1"/>
       <c r="F8" s="1"/>
-      <c r="K8" s="1"/>
-      <c r="L8" s="1"/>
-      <c r="M8" s="1"/>
-    </row>
-    <row r="9" spans="1:14" x14ac:dyDescent="0.15">
+    </row>
+    <row r="9" spans="1:10" x14ac:dyDescent="0.15">
       <c r="A9" s="1"/>
       <c r="B9" s="1"/>
       <c r="C9" s="1"/>
       <c r="E9" s="1"/>
       <c r="F9" s="1"/>
-      <c r="K9" s="1"/>
-      <c r="L9" s="1"/>
-      <c r="M9" s="1"/>
-    </row>
-    <row r="10" spans="1:14" x14ac:dyDescent="0.15">
+    </row>
+    <row r="10" spans="1:10" x14ac:dyDescent="0.15">
       <c r="A10" s="1"/>
       <c r="B10" s="1"/>
     </row>
-    <row r="11" spans="1:14" x14ac:dyDescent="0.15">
+    <row r="11" spans="1:10" x14ac:dyDescent="0.15">
       <c r="A11" s="1"/>
       <c r="B11" s="1"/>
       <c r="C11" s="1"/>
       <c r="E11" s="1"/>
       <c r="F11" s="1"/>
-      <c r="K11" s="1"/>
-      <c r="L11" s="1"/>
-      <c r="M11" s="1"/>
-    </row>
-    <row r="12" spans="1:14" x14ac:dyDescent="0.15">
+    </row>
+    <row r="12" spans="1:10" x14ac:dyDescent="0.15">
       <c r="A12" s="1"/>
       <c r="B12" s="1"/>
       <c r="C12" s="1"/>
       <c r="E12" s="1"/>
       <c r="F12" s="1"/>
-      <c r="K12" s="1"/>
-      <c r="L12" s="1"/>
-      <c r="M12" s="1"/>
-    </row>
-    <row r="13" spans="1:14" x14ac:dyDescent="0.15">
+    </row>
+    <row r="13" spans="1:10" x14ac:dyDescent="0.15">
       <c r="A13" s="1"/>
       <c r="B13" s="1"/>
     </row>
-    <row r="14" spans="1:14" x14ac:dyDescent="0.15">
+    <row r="14" spans="1:10" x14ac:dyDescent="0.15">
       <c r="A14" s="1"/>
       <c r="B14" s="1"/>
       <c r="C14" s="1"/>
       <c r="E14" s="1"/>
       <c r="F14" s="1"/>
-      <c r="K14" s="1"/>
-      <c r="L14" s="1"/>
-      <c r="M14" s="1"/>
-    </row>
-    <row r="15" spans="1:14" x14ac:dyDescent="0.15">
+    </row>
+    <row r="15" spans="1:10" x14ac:dyDescent="0.15">
       <c r="A15" s="1"/>
       <c r="B15" s="1"/>
       <c r="C15" s="1"/>
       <c r="E15" s="1"/>
       <c r="F15" s="1"/>
-      <c r="K15" s="1"/>
-      <c r="L15" s="1"/>
-      <c r="M15" s="1"/>
-    </row>
-    <row r="16" spans="1:14" x14ac:dyDescent="0.15">
+    </row>
+    <row r="16" spans="1:10" x14ac:dyDescent="0.15">
       <c r="A16" s="1"/>
       <c r="B16" s="1"/>
     </row>
-    <row r="17" spans="1:13" x14ac:dyDescent="0.15">
+    <row r="17" spans="1:6" x14ac:dyDescent="0.15">
       <c r="A17" s="1"/>
       <c r="B17" s="1"/>
       <c r="C17" s="1"/>
       <c r="E17" s="1"/>
       <c r="F17" s="1"/>
-      <c r="K17" s="1"/>
-      <c r="L17" s="1"/>
-      <c r="M17" s="1"/>
-    </row>
-    <row r="18" spans="1:13" x14ac:dyDescent="0.15">
+    </row>
+    <row r="18" spans="1:6" x14ac:dyDescent="0.15">
       <c r="A18" s="1"/>
       <c r="B18" s="1"/>
       <c r="C18" s="1"/>
       <c r="E18" s="1"/>
       <c r="F18" s="1"/>
-      <c r="K18" s="1"/>
-      <c r="L18" s="1"/>
-      <c r="M18" s="1"/>
-    </row>
-    <row r="19" spans="1:13" x14ac:dyDescent="0.15">
+    </row>
+    <row r="19" spans="1:6" x14ac:dyDescent="0.15">
       <c r="A19" s="1"/>
       <c r="B19" s="1"/>
     </row>
-    <row r="20" spans="1:13" x14ac:dyDescent="0.15">
+    <row r="20" spans="1:6" x14ac:dyDescent="0.15">
       <c r="A20" s="1"/>
       <c r="B20" s="1"/>
       <c r="C20" s="1"/>
       <c r="E20" s="1"/>
       <c r="F20" s="1"/>
-      <c r="K20" s="1"/>
-      <c r="L20" s="1"/>
-      <c r="M20" s="1"/>
-    </row>
-    <row r="21" spans="1:13" x14ac:dyDescent="0.15">
+    </row>
+    <row r="21" spans="1:6" x14ac:dyDescent="0.15">
       <c r="A21" s="1"/>
       <c r="B21" s="1"/>
       <c r="C21" s="1"/>
       <c r="E21" s="1"/>
       <c r="F21" s="1"/>
-      <c r="K21" s="1"/>
-      <c r="L21" s="1"/>
-      <c r="M21" s="1"/>
-    </row>
-    <row r="22" spans="1:13" x14ac:dyDescent="0.15">
+    </row>
+    <row r="22" spans="1:6" x14ac:dyDescent="0.15">
       <c r="A22" s="1"/>
       <c r="B22" s="1"/>
     </row>
-    <row r="23" spans="1:13" x14ac:dyDescent="0.15">
+    <row r="23" spans="1:6" x14ac:dyDescent="0.15">
       <c r="A23" s="1"/>
       <c r="B23" s="1"/>
       <c r="C23" s="1"/>
       <c r="E23" s="1"/>
       <c r="F23" s="1"/>
-      <c r="K23" s="1"/>
-      <c r="L23" s="1"/>
-      <c r="M23" s="1"/>
-    </row>
-    <row r="24" spans="1:13" x14ac:dyDescent="0.15">
+    </row>
+    <row r="24" spans="1:6" x14ac:dyDescent="0.15">
       <c r="A24" s="1"/>
       <c r="B24" s="1"/>
       <c r="C24" s="1"/>
       <c r="E24" s="1"/>
       <c r="F24" s="1"/>
-      <c r="K24" s="1"/>
-      <c r="L24" s="1"/>
-      <c r="M24" s="1"/>
-    </row>
-    <row r="25" spans="1:13" x14ac:dyDescent="0.15">
+    </row>
+    <row r="25" spans="1:6" x14ac:dyDescent="0.15">
       <c r="A25" s="1"/>
       <c r="B25" s="1"/>
     </row>
-    <row r="26" spans="1:13" x14ac:dyDescent="0.15">
+    <row r="26" spans="1:6" x14ac:dyDescent="0.15">
       <c r="A26" s="1"/>
       <c r="B26" s="1"/>
       <c r="C26" s="1"/>
       <c r="E26" s="1"/>
       <c r="F26" s="1"/>
-      <c r="K26" s="1"/>
-      <c r="L26" s="1"/>
-      <c r="M26" s="1"/>
-    </row>
-    <row r="27" spans="1:13" x14ac:dyDescent="0.15">
+    </row>
+    <row r="27" spans="1:6" x14ac:dyDescent="0.15">
       <c r="A27" s="1"/>
       <c r="B27" s="1"/>
       <c r="C27" s="1"/>
       <c r="E27" s="1"/>
       <c r="F27" s="1"/>
-      <c r="K27" s="1"/>
-      <c r="L27" s="1"/>
-      <c r="M27" s="1"/>
-    </row>
-    <row r="28" spans="1:13" x14ac:dyDescent="0.15">
+    </row>
+    <row r="28" spans="1:6" x14ac:dyDescent="0.15">
       <c r="A28" s="1"/>
       <c r="B28" s="1"/>
     </row>
-    <row r="29" spans="1:13" x14ac:dyDescent="0.15">
+    <row r="29" spans="1:6" x14ac:dyDescent="0.15">
       <c r="A29" s="1"/>
       <c r="B29" s="1"/>
       <c r="C29" s="1"/>
       <c r="E29" s="1"/>
       <c r="F29" s="1"/>
-      <c r="K29" s="1"/>
-      <c r="L29" s="1"/>
-      <c r="M29" s="1"/>
-    </row>
-    <row r="30" spans="1:13" x14ac:dyDescent="0.15">
+    </row>
+    <row r="30" spans="1:6" x14ac:dyDescent="0.15">
       <c r="A30" s="1"/>
       <c r="B30" s="1"/>
       <c r="C30" s="1"/>
       <c r="E30" s="1"/>
       <c r="F30" s="1"/>
-      <c r="K30" s="1"/>
-      <c r="L30" s="1"/>
-      <c r="M30" s="1"/>
-    </row>
-    <row r="31" spans="1:13" x14ac:dyDescent="0.15">
+    </row>
+    <row r="31" spans="1:6" x14ac:dyDescent="0.15">
       <c r="A31" s="1"/>
       <c r="B31" s="1"/>
     </row>
-    <row r="32" spans="1:13" x14ac:dyDescent="0.15">
+    <row r="32" spans="1:6" x14ac:dyDescent="0.15">
       <c r="A32" s="1"/>
       <c r="B32" s="1"/>
       <c r="C32" s="1"/>
       <c r="E32" s="1"/>
       <c r="F32" s="1"/>
-      <c r="K32" s="1"/>
-      <c r="L32" s="1"/>
-      <c r="M32" s="1"/>
-    </row>
-    <row r="33" spans="1:13" x14ac:dyDescent="0.15">
+    </row>
+    <row r="33" spans="1:6" x14ac:dyDescent="0.15">
       <c r="A33" s="1"/>
       <c r="B33" s="1"/>
       <c r="C33" s="1"/>
       <c r="E33" s="1"/>
       <c r="F33" s="1"/>
-      <c r="K33" s="1"/>
-      <c r="L33" s="1"/>
-      <c r="M33" s="1"/>
-    </row>
-    <row r="34" spans="1:13" x14ac:dyDescent="0.15">
+    </row>
+    <row r="34" spans="1:6" x14ac:dyDescent="0.15">
       <c r="A34" s="1"/>
       <c r="B34" s="1"/>
     </row>
-    <row r="35" spans="1:13" x14ac:dyDescent="0.15">
+    <row r="35" spans="1:6" x14ac:dyDescent="0.15">
       <c r="A35" s="1"/>
       <c r="B35" s="1"/>
       <c r="C35" s="1"/>
       <c r="E35" s="1"/>
       <c r="F35" s="1"/>
-      <c r="K35" s="1"/>
-      <c r="L35" s="1"/>
-      <c r="M35" s="1"/>
-    </row>
-    <row r="36" spans="1:13" x14ac:dyDescent="0.15">
+    </row>
+    <row r="36" spans="1:6" x14ac:dyDescent="0.15">
       <c r="A36" s="1"/>
       <c r="B36" s="1"/>
       <c r="C36" s="1"/>
       <c r="E36" s="1"/>
       <c r="F36" s="1"/>
-      <c r="K36" s="1"/>
-      <c r="L36" s="1"/>
-      <c r="M36" s="1"/>
-    </row>
-    <row r="37" spans="1:13" x14ac:dyDescent="0.15">
+    </row>
+    <row r="37" spans="1:6" x14ac:dyDescent="0.15">
       <c r="A37" s="1"/>
       <c r="B37" s="1"/>
     </row>
-    <row r="38" spans="1:13" x14ac:dyDescent="0.15">
+    <row r="38" spans="1:6" x14ac:dyDescent="0.15">
       <c r="A38" s="1"/>
       <c r="B38" s="1"/>
       <c r="C38" s="1"/>
       <c r="E38" s="1"/>
       <c r="F38" s="1"/>
-      <c r="K38" s="1"/>
-      <c r="L38" s="1"/>
-      <c r="M38" s="1"/>
-    </row>
-    <row r="39" spans="1:13" x14ac:dyDescent="0.15">
+    </row>
+    <row r="39" spans="1:6" x14ac:dyDescent="0.15">
       <c r="A39" s="1"/>
       <c r="B39" s="1"/>
       <c r="C39" s="1"/>
       <c r="E39" s="1"/>
       <c r="F39" s="1"/>
-      <c r="K39" s="1"/>
-      <c r="L39" s="1"/>
-      <c r="M39" s="1"/>
-    </row>
-    <row r="40" spans="1:13" x14ac:dyDescent="0.15">
+    </row>
+    <row r="40" spans="1:6" x14ac:dyDescent="0.15">
       <c r="A40" s="1"/>
       <c r="B40" s="1"/>
     </row>
-    <row r="41" spans="1:13" x14ac:dyDescent="0.15">
+    <row r="41" spans="1:6" x14ac:dyDescent="0.15">
       <c r="A41" s="1"/>
       <c r="B41" s="1"/>
       <c r="C41" s="1"/>
       <c r="E41" s="1"/>
       <c r="F41" s="1"/>
-      <c r="K41" s="1"/>
-      <c r="L41" s="1"/>
-      <c r="M41" s="1"/>
-    </row>
-    <row r="42" spans="1:13" x14ac:dyDescent="0.15">
+    </row>
+    <row r="42" spans="1:6" x14ac:dyDescent="0.15">
       <c r="A42" s="1"/>
       <c r="B42" s="1"/>
       <c r="C42" s="1"/>
       <c r="E42" s="1"/>
       <c r="F42" s="1"/>
-      <c r="K42" s="1"/>
-      <c r="L42" s="1"/>
-      <c r="M42" s="1"/>
-    </row>
-    <row r="43" spans="1:13" x14ac:dyDescent="0.15">
+    </row>
+    <row r="43" spans="1:6" x14ac:dyDescent="0.15">
       <c r="A43" s="1"/>
       <c r="B43" s="1"/>
     </row>
-    <row r="44" spans="1:13" x14ac:dyDescent="0.15">
+    <row r="44" spans="1:6" x14ac:dyDescent="0.15">
       <c r="A44" s="1"/>
       <c r="B44" s="1"/>
       <c r="C44" s="1"/>
       <c r="E44" s="1"/>
       <c r="F44" s="1"/>
-      <c r="K44" s="1"/>
-      <c r="L44" s="1"/>
-      <c r="M44" s="1"/>
-    </row>
-    <row r="45" spans="1:13" x14ac:dyDescent="0.15">
+    </row>
+    <row r="45" spans="1:6" x14ac:dyDescent="0.15">
       <c r="A45" s="1"/>
       <c r="B45" s="1"/>
       <c r="C45" s="1"/>
       <c r="E45" s="1"/>
       <c r="F45" s="1"/>
-      <c r="K45" s="1"/>
-      <c r="L45" s="1"/>
-      <c r="M45" s="1"/>
-    </row>
-    <row r="46" spans="1:13" x14ac:dyDescent="0.15">
+    </row>
+    <row r="46" spans="1:6" x14ac:dyDescent="0.15">
       <c r="A46" s="1"/>
       <c r="B46" s="1"/>
     </row>
-    <row r="47" spans="1:13" x14ac:dyDescent="0.15">
+    <row r="47" spans="1:6" x14ac:dyDescent="0.15">
       <c r="A47" s="1"/>
       <c r="B47" s="1"/>
       <c r="C47" s="1"/>
       <c r="E47" s="1"/>
       <c r="F47" s="1"/>
-      <c r="K47" s="1"/>
-      <c r="L47" s="1"/>
-      <c r="M47" s="1"/>
-    </row>
-    <row r="48" spans="1:13" x14ac:dyDescent="0.15">
+    </row>
+    <row r="48" spans="1:6" x14ac:dyDescent="0.15">
       <c r="A48" s="1"/>
       <c r="B48" s="1"/>
       <c r="C48" s="1"/>
       <c r="E48" s="1"/>
       <c r="F48" s="1"/>
-      <c r="K48" s="1"/>
-      <c r="L48" s="1"/>
-      <c r="M48" s="1"/>
-    </row>
-    <row r="49" spans="1:13" x14ac:dyDescent="0.15">
+    </row>
+    <row r="49" spans="1:6" x14ac:dyDescent="0.15">
       <c r="A49" s="1"/>
       <c r="B49" s="1"/>
     </row>
-    <row r="50" spans="1:13" x14ac:dyDescent="0.15">
+    <row r="50" spans="1:6" x14ac:dyDescent="0.15">
       <c r="A50" s="1"/>
       <c r="B50" s="1"/>
       <c r="C50" s="1"/>
       <c r="E50" s="1"/>
       <c r="F50" s="1"/>
-      <c r="K50" s="1"/>
-      <c r="L50" s="1"/>
-      <c r="M50" s="1"/>
-    </row>
-    <row r="51" spans="1:13" x14ac:dyDescent="0.15">
+    </row>
+    <row r="51" spans="1:6" x14ac:dyDescent="0.15">
       <c r="A51" s="1"/>
       <c r="B51" s="1"/>
       <c r="C51" s="1"/>
       <c r="E51" s="1"/>
       <c r="F51" s="1"/>
-      <c r="K51" s="1"/>
-      <c r="L51" s="1"/>
-      <c r="M51" s="1"/>
-    </row>
-    <row r="52" spans="1:13" x14ac:dyDescent="0.15">
+    </row>
+    <row r="52" spans="1:6" x14ac:dyDescent="0.15">
       <c r="A52" s="1"/>
       <c r="B52" s="1"/>
     </row>
-    <row r="53" spans="1:13" x14ac:dyDescent="0.15">
+    <row r="53" spans="1:6" x14ac:dyDescent="0.15">
       <c r="A53" s="1"/>
       <c r="B53" s="1"/>
       <c r="C53" s="1"/>
       <c r="E53" s="1"/>
       <c r="F53" s="1"/>
-      <c r="K53" s="1"/>
-      <c r="L53" s="1"/>
-      <c r="M53" s="1"/>
     </row>
   </sheetData>
   <phoneticPr fontId="1" type="noConversion"/>

</xml_diff>

<commit_message>
add property for block
</commit_message>
<xml_diff>
--- a/_Out/Server/NFDataCfg/Excel_Ini/Block.xlsx
+++ b/_Out/Server/NFDataCfg/Excel_Ini/Block.xlsx
@@ -27,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="10" uniqueCount="10">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="22" uniqueCount="22">
   <si>
     <t>ID</t>
     <phoneticPr fontId="1" type="noConversion"/>
@@ -67,6 +67,48 @@
   <si>
     <t>Tag</t>
     <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Grass1</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Grass2</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Grass3</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Grass4</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Grass5</t>
+  </si>
+  <si>
+    <t>Crack1</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Crack2</t>
+  </si>
+  <si>
+    <t>Crack3</t>
+  </si>
+  <si>
+    <t>Crack4</t>
+  </si>
+  <si>
+    <t>Crack5</t>
+  </si>
+  <si>
+    <t>Treasure1</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Treasure2</t>
   </si>
 </sst>
 </file>
@@ -176,9 +218,9 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="1" name="表1" displayName="表1" ref="A1:J53" tableType="xml" totalsRowShown="0" connectionId="1">
-  <autoFilter ref="A1:J53"/>
-  <tableColumns count="10">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="1" name="表1" displayName="表1" ref="A1:V53" tableType="xml" totalsRowShown="0" connectionId="1">
+  <autoFilter ref="A1:V53"/>
+  <tableColumns count="22">
     <tableColumn id="1" uniqueName="ID" name="ID">
       <xmlColumnPr mapId="1" xpath="/XML/Object/@ID" xmlDataType="string"/>
     </tableColumn>
@@ -207,6 +249,18 @@
     <tableColumn id="9" uniqueName="AwardGold" name="RightDownSide">
       <xmlColumnPr mapId="1" xpath="/XML/Object/@AwardGold" xmlDataType="integer"/>
     </tableColumn>
+    <tableColumn id="10" uniqueName="10" name="Grass1"/>
+    <tableColumn id="11" uniqueName="11" name="Grass2"/>
+    <tableColumn id="12" uniqueName="12" name="Grass3"/>
+    <tableColumn id="13" uniqueName="13" name="Grass4"/>
+    <tableColumn id="15" uniqueName="15" name="Grass5"/>
+    <tableColumn id="16" uniqueName="16" name="Crack1"/>
+    <tableColumn id="17" uniqueName="17" name="Crack2"/>
+    <tableColumn id="18" uniqueName="18" name="Crack3"/>
+    <tableColumn id="19" uniqueName="19" name="Crack4"/>
+    <tableColumn id="20" uniqueName="20" name="Crack5"/>
+    <tableColumn id="21" uniqueName="21" name="Treasure1"/>
+    <tableColumn id="22" uniqueName="22" name="Treasure2"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -475,10 +529,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:J53"/>
+  <dimension ref="A1:V53"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="B1" workbookViewId="0">
-      <selection activeCell="K1" sqref="K1:K1048576"/>
+    <sheetView tabSelected="1" topLeftCell="I1" workbookViewId="0">
+      <selection activeCell="U7" sqref="U7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.5" x14ac:dyDescent="0.15"/>
@@ -491,10 +545,17 @@
     <col min="7" max="7" width="14" bestFit="1" customWidth="1"/>
     <col min="8" max="8" width="24.625" customWidth="1"/>
     <col min="9" max="9" width="27" customWidth="1"/>
-    <col min="10" max="10" width="14" bestFit="1" customWidth="1"/>
+    <col min="10" max="11" width="14" bestFit="1" customWidth="1"/>
+    <col min="12" max="13" width="15.25" customWidth="1"/>
+    <col min="14" max="14" width="15.75" customWidth="1"/>
+    <col min="15" max="15" width="13.875" customWidth="1"/>
+    <col min="16" max="16" width="17.125" customWidth="1"/>
+    <col min="17" max="19" width="10.5" bestFit="1" customWidth="1"/>
+    <col min="21" max="21" width="16.375" customWidth="1"/>
+    <col min="22" max="22" width="15.375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:10" x14ac:dyDescent="0.15">
+    <row r="1" spans="1:22" x14ac:dyDescent="0.15">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -525,94 +586,130 @@
       <c r="J1" t="s">
         <v>8</v>
       </c>
-    </row>
-    <row r="2" spans="1:10" x14ac:dyDescent="0.15">
+      <c r="K1" t="s">
+        <v>10</v>
+      </c>
+      <c r="L1" t="s">
+        <v>11</v>
+      </c>
+      <c r="M1" t="s">
+        <v>12</v>
+      </c>
+      <c r="N1" t="s">
+        <v>13</v>
+      </c>
+      <c r="O1" t="s">
+        <v>14</v>
+      </c>
+      <c r="P1" t="s">
+        <v>15</v>
+      </c>
+      <c r="Q1" t="s">
+        <v>16</v>
+      </c>
+      <c r="R1" t="s">
+        <v>17</v>
+      </c>
+      <c r="S1" t="s">
+        <v>18</v>
+      </c>
+      <c r="T1" t="s">
+        <v>19</v>
+      </c>
+      <c r="U1" t="s">
+        <v>20</v>
+      </c>
+      <c r="V1" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="2" spans="1:22" x14ac:dyDescent="0.15">
       <c r="A2" s="1"/>
       <c r="B2" s="1"/>
       <c r="C2" s="1"/>
       <c r="E2" s="1"/>
       <c r="F2" s="1"/>
     </row>
-    <row r="3" spans="1:10" x14ac:dyDescent="0.15">
+    <row r="3" spans="1:22" x14ac:dyDescent="0.15">
       <c r="A3" s="1"/>
       <c r="B3" s="1"/>
       <c r="C3" s="1"/>
       <c r="E3" s="1"/>
       <c r="F3" s="1"/>
     </row>
-    <row r="4" spans="1:10" x14ac:dyDescent="0.15">
+    <row r="4" spans="1:22" x14ac:dyDescent="0.15">
       <c r="A4" s="1"/>
       <c r="B4" s="1"/>
     </row>
-    <row r="5" spans="1:10" x14ac:dyDescent="0.15">
+    <row r="5" spans="1:22" x14ac:dyDescent="0.15">
       <c r="A5" s="1"/>
       <c r="B5" s="1"/>
       <c r="C5" s="1"/>
       <c r="E5" s="1"/>
       <c r="F5" s="1"/>
     </row>
-    <row r="6" spans="1:10" x14ac:dyDescent="0.15">
+    <row r="6" spans="1:22" x14ac:dyDescent="0.15">
       <c r="A6" s="1"/>
       <c r="B6" s="1"/>
       <c r="C6" s="1"/>
       <c r="E6" s="1"/>
       <c r="F6" s="1"/>
     </row>
-    <row r="7" spans="1:10" x14ac:dyDescent="0.15">
+    <row r="7" spans="1:22" x14ac:dyDescent="0.15">
       <c r="A7" s="1"/>
       <c r="B7" s="1"/>
     </row>
-    <row r="8" spans="1:10" x14ac:dyDescent="0.15">
+    <row r="8" spans="1:22" x14ac:dyDescent="0.15">
       <c r="A8" s="1"/>
       <c r="B8" s="1"/>
       <c r="C8" s="1"/>
       <c r="E8" s="1"/>
       <c r="F8" s="1"/>
     </row>
-    <row r="9" spans="1:10" x14ac:dyDescent="0.15">
+    <row r="9" spans="1:22" x14ac:dyDescent="0.15">
       <c r="A9" s="1"/>
       <c r="B9" s="1"/>
       <c r="C9" s="1"/>
       <c r="E9" s="1"/>
       <c r="F9" s="1"/>
     </row>
-    <row r="10" spans="1:10" x14ac:dyDescent="0.15">
+    <row r="10" spans="1:22" x14ac:dyDescent="0.15">
       <c r="A10" s="1"/>
       <c r="B10" s="1"/>
     </row>
-    <row r="11" spans="1:10" x14ac:dyDescent="0.15">
+    <row r="11" spans="1:22" x14ac:dyDescent="0.15">
       <c r="A11" s="1"/>
       <c r="B11" s="1"/>
       <c r="C11" s="1"/>
       <c r="E11" s="1"/>
       <c r="F11" s="1"/>
     </row>
-    <row r="12" spans="1:10" x14ac:dyDescent="0.15">
+    <row r="12" spans="1:22" x14ac:dyDescent="0.15">
       <c r="A12" s="1"/>
       <c r="B12" s="1"/>
       <c r="C12" s="1"/>
       <c r="E12" s="1"/>
       <c r="F12" s="1"/>
     </row>
-    <row r="13" spans="1:10" x14ac:dyDescent="0.15">
+    <row r="13" spans="1:22" x14ac:dyDescent="0.15">
       <c r="A13" s="1"/>
       <c r="B13" s="1"/>
     </row>
-    <row r="14" spans="1:10" x14ac:dyDescent="0.15">
+    <row r="14" spans="1:22" x14ac:dyDescent="0.15">
       <c r="A14" s="1"/>
       <c r="B14" s="1"/>
       <c r="C14" s="1"/>
       <c r="E14" s="1"/>
       <c r="F14" s="1"/>
     </row>
-    <row r="15" spans="1:10" x14ac:dyDescent="0.15">
+    <row r="15" spans="1:22" x14ac:dyDescent="0.15">
       <c r="A15" s="1"/>
       <c r="B15" s="1"/>
       <c r="C15" s="1"/>
       <c r="E15" s="1"/>
       <c r="F15" s="1"/>
     </row>
-    <row r="16" spans="1:10" x14ac:dyDescent="0.15">
+    <row r="16" spans="1:22" x14ac:dyDescent="0.15">
       <c r="A16" s="1"/>
       <c r="B16" s="1"/>
     </row>

</xml_diff>

<commit_message>
remove struct about excel move struct to ini
</commit_message>
<xml_diff>
--- a/_Out/Server/NFDataCfg/Excel_Ini/Block.xlsx
+++ b/_Out/Server/NFDataCfg/Excel_Ini/Block.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="3" lowestEdited="5" rupBuild="9302"/>
   <workbookPr/>
   <bookViews>
-    <workbookView windowWidth="28695" windowHeight="13050"/>
+    <workbookView windowWidth="19455" windowHeight="9990"/>
   </bookViews>
   <sheets>
     <sheet name="Property1" sheetId="1" r:id="rId1"/>
@@ -287,12 +287,12 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <numFmts count="4">
-    <numFmt numFmtId="42" formatCode="_ &quot;￥&quot;* #,##0_ ;_ &quot;￥&quot;* \-#,##0_ ;_ &quot;￥&quot;* &quot;-&quot;_ ;_ @_ "/>
-    <numFmt numFmtId="44" formatCode="_ &quot;￥&quot;* #,##0.00_ ;_ &quot;￥&quot;* \-#,##0.00_ ;_ &quot;￥&quot;* &quot;-&quot;??_ ;_ @_ "/>
-    <numFmt numFmtId="43" formatCode="_ * #,##0.00_ ;_ * \-#,##0.00_ ;_ * &quot;-&quot;??_ ;_ @_ "/>
-    <numFmt numFmtId="41" formatCode="_ * #,##0_ ;_ * \-#,##0_ ;_ * &quot;-&quot;_ ;_ @_ "/>
+    <numFmt numFmtId="176" formatCode="_ &quot;￥&quot;* #,##0.00_ ;_ &quot;￥&quot;* \-#,##0.00_ ;_ &quot;￥&quot;* &quot;-&quot;??_ ;_ @_ "/>
+    <numFmt numFmtId="177" formatCode="_ * #,##0_ ;_ * \-#,##0_ ;_ * &quot;-&quot;_ ;_ @_ "/>
+    <numFmt numFmtId="178" formatCode="_ * #,##0.00_ ;_ * \-#,##0.00_ ;_ * &quot;-&quot;??_ ;_ @_ "/>
+    <numFmt numFmtId="179" formatCode="_ &quot;￥&quot;* #,##0_ ;_ &quot;￥&quot;* \-#,##0_ ;_ &quot;￥&quot;* &quot;-&quot;_ ;_ @_ "/>
   </numFmts>
-  <fonts count="21">
+  <fonts count="22">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -301,6 +301,15 @@
       <scheme val="minor"/>
     </font>
     <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="宋体"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
       <sz val="11"/>
       <color indexed="8"/>
       <name val="宋体"/>
@@ -321,90 +330,6 @@
       <scheme val="minor"/>
     </font>
     <font>
-      <b/>
-      <sz val="11"/>
-      <color rgb="FFFA7D00"/>
-      <name val="宋体"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="18"/>
-      <color theme="3"/>
-      <name val="宋体"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <u/>
-      <sz val="11"/>
-      <color rgb="FF0000FF"/>
-      <name val="宋体"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF9C0006"/>
-      <name val="宋体"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF9C6500"/>
-      <name val="宋体"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FFFA7D00"/>
-      <name val="宋体"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="15"/>
-      <color theme="3"/>
-      <name val="宋体"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color theme="1"/>
-      <name val="宋体"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF006100"/>
-      <name val="宋体"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color rgb="FFFFFFFF"/>
-      <name val="宋体"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="13"/>
-      <color theme="3"/>
-      <name val="宋体"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
       <sz val="11"/>
       <color rgb="FFFF0000"/>
       <name val="宋体"/>
@@ -421,7 +346,7 @@
     <font>
       <b/>
       <sz val="11"/>
-      <color rgb="FF3F3F3F"/>
+      <color theme="1"/>
       <name val="宋体"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -429,15 +354,7 @@
     <font>
       <b/>
       <sz val="11"/>
-      <color theme="3"/>
-      <name val="宋体"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <i/>
-      <sz val="11"/>
-      <color rgb="FF7F7F7F"/>
+      <color rgb="FFFA7D00"/>
       <name val="宋体"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -450,6 +367,98 @@
       <charset val="0"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF9C0006"/>
+      <name val="宋体"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FFFA7D00"/>
+      <name val="宋体"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF9C6500"/>
+      <name val="宋体"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF006100"/>
+      <name val="宋体"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="15"/>
+      <color theme="3"/>
+      <name val="宋体"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="18"/>
+      <color theme="3"/>
+      <name val="宋体"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="3"/>
+      <name val="宋体"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="11"/>
+      <color rgb="FF0000FF"/>
+      <name val="宋体"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FFFFFFFF"/>
+      <name val="宋体"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <i/>
+      <sz val="11"/>
+      <color rgb="FF7F7F7F"/>
+      <name val="宋体"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FF3F3F3F"/>
+      <name val="宋体"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="13"/>
+      <color theme="3"/>
+      <name val="宋体"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
   <fills count="35">
     <fill>
@@ -472,197 +481,287 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFCC99"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFF2F2F2"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFC7CE"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFEB9C"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFC6EFCE"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFFCC"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFA5A5A5"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
         <fgColor theme="9" tint="0.599993896298105"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="9"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFF2F2F2"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFC7CE"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFEB9C"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFFFCC"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFC6EFCE"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFA5A5A5"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFCC99"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
         <fgColor theme="9" tint="0.399975585192419"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
   </fills>
-  <borders count="9">
+  <borders count="15">
     <border>
       <left/>
       <right/>
       <top/>
       <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color auto="1"/>
+      </left>
+      <right style="thin">
+        <color auto="1"/>
+      </right>
+      <top style="medium">
+        <color auto="1"/>
+      </top>
+      <bottom style="thin">
+        <color auto="1"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color auto="1"/>
+      </left>
+      <right style="thin">
+        <color auto="1"/>
+      </right>
+      <top style="thin">
+        <color auto="1"/>
+      </top>
+      <bottom style="thin">
+        <color auto="1"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color auto="1"/>
+      </left>
+      <right style="thin">
+        <color auto="1"/>
+      </right>
+      <top style="thin">
+        <color auto="1"/>
+      </top>
+      <bottom style="medium">
+        <color auto="1"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color auto="1"/>
+      </left>
+      <right style="thin">
+        <color auto="1"/>
+      </right>
+      <top style="medium">
+        <color auto="1"/>
+      </top>
+      <bottom style="thin">
+        <color auto="1"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color auto="1"/>
+      </left>
+      <right style="thin">
+        <color auto="1"/>
+      </right>
+      <top style="thin">
+        <color auto="1"/>
+      </top>
+      <bottom style="thin">
+        <color auto="1"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color auto="1"/>
+      </left>
+      <right style="thin">
+        <color auto="1"/>
+      </right>
+      <top style="thin">
+        <color auto="1"/>
+      </top>
+      <bottom style="medium">
+        <color auto="1"/>
+      </bottom>
       <diagonal/>
     </border>
     <border>
@@ -677,6 +776,17 @@
       </top>
       <bottom style="thin">
         <color rgb="FF7F7F7F"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top style="thin">
+        <color theme="4"/>
+      </top>
+      <bottom style="double">
+        <color theme="4"/>
       </bottom>
       <diagonal/>
     </border>
@@ -714,17 +824,6 @@
       <diagonal/>
     </border>
     <border>
-      <left/>
-      <right/>
-      <top style="thin">
-        <color theme="4"/>
-      </top>
-      <bottom style="double">
-        <color theme="4"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
       <left style="double">
         <color rgb="FF3F3F3F"/>
       </left>
@@ -736,6 +835,15 @@
       </top>
       <bottom style="double">
         <color rgb="FF3F3F3F"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="medium">
+        <color theme="4" tint="0.499984740745262"/>
       </bottom>
       <diagonal/>
     </border>
@@ -754,189 +862,195 @@
       </bottom>
       <diagonal/>
     </border>
-    <border>
-      <left/>
-      <right/>
-      <top/>
-      <bottom style="medium">
-        <color theme="4" tint="0.499984740745262"/>
-      </bottom>
-      <diagonal/>
-    </border>
   </borders>
   <cellStyleXfs count="49">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="42" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="29" borderId="1" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="44" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="41" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="43" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="179" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="7" borderId="7" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="176" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="177" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="178" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="9" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="20" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="16" borderId="4" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="18" borderId="11" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="6" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="10" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="21" fillId="0" borderId="10" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="13" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="5" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="10" borderId="14" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="10" borderId="7" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="24" borderId="12" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="9" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="8" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="4" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="9" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="18" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="3" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="3" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="0" borderId="8" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="4" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="17" fillId="8" borderId="7" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="8" borderId="1" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="24" borderId="6" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="2" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="5" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="7" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="6" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="34" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="33" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="9" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="5" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="4" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="4" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="8" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="33" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="34" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="8">
+  <cellXfs count="13">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1">
-      <alignment vertical="center"/>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="49" fontId="1" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="49" fontId="1" fillId="3" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="2" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="2" fillId="3" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="2" fillId="3" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="49">
@@ -1255,15 +1369,15 @@
   <sheetPr/>
   <dimension ref="A1:U22"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C29" sqref="C29"/>
+    <sheetView tabSelected="1" topLeftCell="O1" workbookViewId="0">
+      <selection activeCell="A7" sqref="$A1:$XFD7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="13.5"/>
   <cols>
     <col min="1" max="1" width="27.375" customWidth="1"/>
     <col min="2" max="2" width="17.375" customWidth="1"/>
-    <col min="3" max="3" width="56" style="3" customWidth="1"/>
+    <col min="3" max="3" width="13" style="4" customWidth="1"/>
     <col min="4" max="4" width="17.375" customWidth="1"/>
     <col min="5" max="5" width="12.75" customWidth="1"/>
     <col min="6" max="6" width="14" customWidth="1"/>
@@ -1282,419 +1396,419 @@
   </cols>
   <sheetData>
     <row r="1" s="1" customFormat="1" spans="1:21">
-      <c r="A1" s="4" t="s">
-        <v>0</v>
-      </c>
-      <c r="B1" s="5" t="s">
+      <c r="A1" s="5" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="6" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="5" t="s">
+      <c r="C1" s="6" t="s">
         <v>2</v>
       </c>
-      <c r="D1" s="5" t="s">
+      <c r="D1" s="6" t="s">
         <v>3</v>
       </c>
-      <c r="E1" s="5" t="s">
+      <c r="E1" s="6" t="s">
         <v>4</v>
       </c>
-      <c r="F1" s="5" t="s">
+      <c r="F1" s="6" t="s">
         <v>5</v>
       </c>
-      <c r="G1" s="5" t="s">
+      <c r="G1" s="6" t="s">
         <v>6</v>
       </c>
-      <c r="H1" s="5" t="s">
+      <c r="H1" s="6" t="s">
         <v>7</v>
       </c>
-      <c r="I1" s="5" t="s">
+      <c r="I1" s="6" t="s">
         <v>8</v>
       </c>
-      <c r="J1" s="5" t="s">
+      <c r="J1" s="6" t="s">
         <v>9</v>
       </c>
-      <c r="K1" s="5" t="s">
+      <c r="K1" s="6" t="s">
         <v>10</v>
       </c>
-      <c r="L1" s="5" t="s">
+      <c r="L1" s="6" t="s">
         <v>11</v>
       </c>
-      <c r="M1" s="5" t="s">
+      <c r="M1" s="6" t="s">
         <v>12</v>
       </c>
-      <c r="N1" s="5" t="s">
+      <c r="N1" s="6" t="s">
         <v>13</v>
       </c>
-      <c r="O1" s="5" t="s">
+      <c r="O1" s="6" t="s">
         <v>14</v>
       </c>
-      <c r="P1" s="5" t="s">
+      <c r="P1" s="6" t="s">
         <v>15</v>
       </c>
-      <c r="Q1" s="5" t="s">
+      <c r="Q1" s="6" t="s">
         <v>16</v>
       </c>
-      <c r="R1" s="5" t="s">
+      <c r="R1" s="6" t="s">
         <v>17</v>
       </c>
-      <c r="S1" s="5" t="s">
+      <c r="S1" s="6" t="s">
         <v>18</v>
       </c>
-      <c r="T1" s="5" t="s">
+      <c r="T1" s="6" t="s">
         <v>19</v>
       </c>
-      <c r="U1" s="5" t="s">
+      <c r="U1" s="6" t="s">
         <v>20</v>
       </c>
     </row>
     <row r="2" s="2" customFormat="1" spans="1:21">
-      <c r="A2" s="6" t="s">
+      <c r="A2" s="7" t="s">
         <v>21</v>
       </c>
-      <c r="B2" s="7" t="s">
+      <c r="B2" s="8" t="s">
         <v>22</v>
       </c>
-      <c r="C2" s="7" t="s">
+      <c r="C2" s="8" t="s">
         <v>23</v>
       </c>
-      <c r="D2" s="7" t="s">
+      <c r="D2" s="8" t="s">
         <v>23</v>
       </c>
-      <c r="E2" s="7" t="s">
+      <c r="E2" s="8" t="s">
         <v>23</v>
       </c>
-      <c r="F2" s="7" t="s">
+      <c r="F2" s="8" t="s">
         <v>23</v>
       </c>
-      <c r="G2" s="7" t="s">
+      <c r="G2" s="8" t="s">
         <v>23</v>
       </c>
-      <c r="H2" s="7" t="s">
+      <c r="H2" s="8" t="s">
         <v>23</v>
       </c>
-      <c r="I2" s="7" t="s">
+      <c r="I2" s="8" t="s">
         <v>23</v>
       </c>
-      <c r="J2" s="7" t="s">
+      <c r="J2" s="8" t="s">
         <v>23</v>
       </c>
-      <c r="K2" s="7" t="s">
+      <c r="K2" s="8" t="s">
         <v>23</v>
       </c>
-      <c r="L2" s="7" t="s">
+      <c r="L2" s="8" t="s">
         <v>23</v>
       </c>
-      <c r="M2" s="7" t="s">
+      <c r="M2" s="8" t="s">
         <v>23</v>
       </c>
-      <c r="N2" s="7" t="s">
+      <c r="N2" s="8" t="s">
         <v>23</v>
       </c>
-      <c r="O2" s="7" t="s">
+      <c r="O2" s="8" t="s">
         <v>23</v>
       </c>
-      <c r="P2" s="7" t="s">
+      <c r="P2" s="8" t="s">
         <v>23</v>
       </c>
-      <c r="Q2" s="7" t="s">
+      <c r="Q2" s="8" t="s">
         <v>23</v>
       </c>
-      <c r="R2" s="7" t="s">
+      <c r="R2" s="8" t="s">
         <v>23</v>
       </c>
-      <c r="S2" s="7" t="s">
+      <c r="S2" s="8" t="s">
         <v>23</v>
       </c>
-      <c r="T2" s="7" t="s">
+      <c r="T2" s="8" t="s">
         <v>23</v>
       </c>
-      <c r="U2" s="7" t="s">
+      <c r="U2" s="8" t="s">
         <v>23</v>
       </c>
     </row>
     <row r="3" s="2" customFormat="1" spans="1:21">
-      <c r="A3" s="6" t="s">
+      <c r="A3" s="7" t="s">
         <v>24</v>
       </c>
-      <c r="B3" s="6" t="b">
-        <v>0</v>
-      </c>
-      <c r="C3" s="6" t="b">
-        <v>0</v>
-      </c>
-      <c r="D3" s="6" t="b">
-        <v>0</v>
-      </c>
-      <c r="E3" s="6" t="b">
-        <v>0</v>
-      </c>
-      <c r="F3" s="6" t="b">
-        <v>0</v>
-      </c>
-      <c r="G3" s="6" t="b">
-        <v>0</v>
-      </c>
-      <c r="H3" s="6" t="b">
-        <v>0</v>
-      </c>
-      <c r="I3" s="6" t="b">
-        <v>0</v>
-      </c>
-      <c r="J3" s="6" t="b">
-        <v>0</v>
-      </c>
-      <c r="K3" s="6" t="b">
-        <v>0</v>
-      </c>
-      <c r="L3" s="6" t="b">
-        <v>0</v>
-      </c>
-      <c r="M3" s="6" t="b">
-        <v>0</v>
-      </c>
-      <c r="N3" s="6" t="b">
-        <v>0</v>
-      </c>
-      <c r="O3" s="6" t="b">
-        <v>0</v>
-      </c>
-      <c r="P3" s="6" t="b">
-        <v>0</v>
-      </c>
-      <c r="Q3" s="6" t="b">
-        <v>0</v>
-      </c>
-      <c r="R3" s="6" t="b">
-        <v>0</v>
-      </c>
-      <c r="S3" s="6" t="b">
-        <v>0</v>
-      </c>
-      <c r="T3" s="6" t="b">
-        <v>0</v>
-      </c>
-      <c r="U3" s="6" t="b">
+      <c r="B3" s="9" t="b">
+        <v>0</v>
+      </c>
+      <c r="C3" s="9" t="b">
+        <v>0</v>
+      </c>
+      <c r="D3" s="9" t="b">
+        <v>0</v>
+      </c>
+      <c r="E3" s="9" t="b">
+        <v>0</v>
+      </c>
+      <c r="F3" s="9" t="b">
+        <v>0</v>
+      </c>
+      <c r="G3" s="9" t="b">
+        <v>0</v>
+      </c>
+      <c r="H3" s="9" t="b">
+        <v>0</v>
+      </c>
+      <c r="I3" s="9" t="b">
+        <v>0</v>
+      </c>
+      <c r="J3" s="9" t="b">
+        <v>0</v>
+      </c>
+      <c r="K3" s="9" t="b">
+        <v>0</v>
+      </c>
+      <c r="L3" s="9" t="b">
+        <v>0</v>
+      </c>
+      <c r="M3" s="9" t="b">
+        <v>0</v>
+      </c>
+      <c r="N3" s="9" t="b">
+        <v>0</v>
+      </c>
+      <c r="O3" s="9" t="b">
+        <v>0</v>
+      </c>
+      <c r="P3" s="9" t="b">
+        <v>0</v>
+      </c>
+      <c r="Q3" s="9" t="b">
+        <v>0</v>
+      </c>
+      <c r="R3" s="9" t="b">
+        <v>0</v>
+      </c>
+      <c r="S3" s="9" t="b">
+        <v>0</v>
+      </c>
+      <c r="T3" s="9" t="b">
+        <v>0</v>
+      </c>
+      <c r="U3" s="9" t="b">
         <v>0</v>
       </c>
     </row>
     <row r="4" s="2" customFormat="1" spans="1:21">
-      <c r="A4" s="6" t="s">
+      <c r="A4" s="7" t="s">
         <v>25</v>
       </c>
-      <c r="B4" s="6" t="b">
-        <v>0</v>
-      </c>
-      <c r="C4" s="6" t="b">
-        <v>0</v>
-      </c>
-      <c r="D4" s="6" t="b">
-        <v>0</v>
-      </c>
-      <c r="E4" s="6" t="b">
-        <v>0</v>
-      </c>
-      <c r="F4" s="6" t="b">
-        <v>0</v>
-      </c>
-      <c r="G4" s="6" t="b">
-        <v>0</v>
-      </c>
-      <c r="H4" s="6" t="b">
-        <v>0</v>
-      </c>
-      <c r="I4" s="6" t="b">
-        <v>0</v>
-      </c>
-      <c r="J4" s="6" t="b">
-        <v>0</v>
-      </c>
-      <c r="K4" s="6" t="b">
-        <v>0</v>
-      </c>
-      <c r="L4" s="6" t="b">
-        <v>0</v>
-      </c>
-      <c r="M4" s="6" t="b">
-        <v>0</v>
-      </c>
-      <c r="N4" s="6" t="b">
-        <v>0</v>
-      </c>
-      <c r="O4" s="6" t="b">
-        <v>0</v>
-      </c>
-      <c r="P4" s="6" t="b">
-        <v>0</v>
-      </c>
-      <c r="Q4" s="6" t="b">
-        <v>0</v>
-      </c>
-      <c r="R4" s="6" t="b">
-        <v>0</v>
-      </c>
-      <c r="S4" s="6" t="b">
-        <v>0</v>
-      </c>
-      <c r="T4" s="6" t="b">
-        <v>0</v>
-      </c>
-      <c r="U4" s="6" t="b">
+      <c r="B4" s="9" t="b">
+        <v>0</v>
+      </c>
+      <c r="C4" s="9" t="b">
+        <v>0</v>
+      </c>
+      <c r="D4" s="9" t="b">
+        <v>0</v>
+      </c>
+      <c r="E4" s="9" t="b">
+        <v>0</v>
+      </c>
+      <c r="F4" s="9" t="b">
+        <v>0</v>
+      </c>
+      <c r="G4" s="9" t="b">
+        <v>0</v>
+      </c>
+      <c r="H4" s="9" t="b">
+        <v>0</v>
+      </c>
+      <c r="I4" s="9" t="b">
+        <v>0</v>
+      </c>
+      <c r="J4" s="9" t="b">
+        <v>0</v>
+      </c>
+      <c r="K4" s="9" t="b">
+        <v>0</v>
+      </c>
+      <c r="L4" s="9" t="b">
+        <v>0</v>
+      </c>
+      <c r="M4" s="9" t="b">
+        <v>0</v>
+      </c>
+      <c r="N4" s="9" t="b">
+        <v>0</v>
+      </c>
+      <c r="O4" s="9" t="b">
+        <v>0</v>
+      </c>
+      <c r="P4" s="9" t="b">
+        <v>0</v>
+      </c>
+      <c r="Q4" s="9" t="b">
+        <v>0</v>
+      </c>
+      <c r="R4" s="9" t="b">
+        <v>0</v>
+      </c>
+      <c r="S4" s="9" t="b">
+        <v>0</v>
+      </c>
+      <c r="T4" s="9" t="b">
+        <v>0</v>
+      </c>
+      <c r="U4" s="9" t="b">
         <v>0</v>
       </c>
     </row>
     <row r="5" s="2" customFormat="1" spans="1:21">
-      <c r="A5" s="6" t="s">
+      <c r="A5" s="7" t="s">
         <v>26</v>
       </c>
-      <c r="B5" s="6" t="b">
-        <v>0</v>
-      </c>
-      <c r="C5" s="6" t="b">
-        <v>0</v>
-      </c>
-      <c r="D5" s="6" t="b">
-        <v>0</v>
-      </c>
-      <c r="E5" s="6" t="b">
-        <v>0</v>
-      </c>
-      <c r="F5" s="6" t="b">
-        <v>0</v>
-      </c>
-      <c r="G5" s="6" t="b">
-        <v>0</v>
-      </c>
-      <c r="H5" s="6" t="b">
-        <v>0</v>
-      </c>
-      <c r="I5" s="6" t="b">
-        <v>0</v>
-      </c>
-      <c r="J5" s="6" t="b">
-        <v>0</v>
-      </c>
-      <c r="K5" s="6" t="b">
-        <v>0</v>
-      </c>
-      <c r="L5" s="6" t="b">
-        <v>0</v>
-      </c>
-      <c r="M5" s="6" t="b">
-        <v>0</v>
-      </c>
-      <c r="N5" s="6" t="b">
-        <v>0</v>
-      </c>
-      <c r="O5" s="6" t="b">
-        <v>0</v>
-      </c>
-      <c r="P5" s="6" t="b">
-        <v>0</v>
-      </c>
-      <c r="Q5" s="6" t="b">
-        <v>0</v>
-      </c>
-      <c r="R5" s="6" t="b">
-        <v>0</v>
-      </c>
-      <c r="S5" s="6" t="b">
-        <v>0</v>
-      </c>
-      <c r="T5" s="6" t="b">
-        <v>0</v>
-      </c>
-      <c r="U5" s="6" t="b">
+      <c r="B5" s="9" t="b">
+        <v>0</v>
+      </c>
+      <c r="C5" s="9" t="b">
+        <v>0</v>
+      </c>
+      <c r="D5" s="9" t="b">
+        <v>0</v>
+      </c>
+      <c r="E5" s="9" t="b">
+        <v>0</v>
+      </c>
+      <c r="F5" s="9" t="b">
+        <v>0</v>
+      </c>
+      <c r="G5" s="9" t="b">
+        <v>0</v>
+      </c>
+      <c r="H5" s="9" t="b">
+        <v>0</v>
+      </c>
+      <c r="I5" s="9" t="b">
+        <v>0</v>
+      </c>
+      <c r="J5" s="9" t="b">
+        <v>0</v>
+      </c>
+      <c r="K5" s="9" t="b">
+        <v>0</v>
+      </c>
+      <c r="L5" s="9" t="b">
+        <v>0</v>
+      </c>
+      <c r="M5" s="9" t="b">
+        <v>0</v>
+      </c>
+      <c r="N5" s="9" t="b">
+        <v>0</v>
+      </c>
+      <c r="O5" s="9" t="b">
+        <v>0</v>
+      </c>
+      <c r="P5" s="9" t="b">
+        <v>0</v>
+      </c>
+      <c r="Q5" s="9" t="b">
+        <v>0</v>
+      </c>
+      <c r="R5" s="9" t="b">
+        <v>0</v>
+      </c>
+      <c r="S5" s="9" t="b">
+        <v>0</v>
+      </c>
+      <c r="T5" s="9" t="b">
+        <v>0</v>
+      </c>
+      <c r="U5" s="9" t="b">
         <v>0</v>
       </c>
     </row>
     <row r="6" s="2" customFormat="1" spans="1:21">
-      <c r="A6" s="6" t="s">
+      <c r="A6" s="7" t="s">
         <v>27</v>
       </c>
-      <c r="B6" s="6" t="b">
-        <v>0</v>
-      </c>
-      <c r="C6" s="6" t="b">
-        <v>0</v>
-      </c>
-      <c r="D6" s="6" t="b">
-        <v>0</v>
-      </c>
-      <c r="E6" s="6" t="b">
-        <v>0</v>
-      </c>
-      <c r="F6" s="6" t="b">
-        <v>0</v>
-      </c>
-      <c r="G6" s="6" t="b">
-        <v>0</v>
-      </c>
-      <c r="H6" s="6" t="b">
-        <v>0</v>
-      </c>
-      <c r="I6" s="6" t="b">
-        <v>0</v>
-      </c>
-      <c r="J6" s="6" t="b">
-        <v>0</v>
-      </c>
-      <c r="K6" s="6" t="b">
-        <v>0</v>
-      </c>
-      <c r="L6" s="6" t="b">
-        <v>0</v>
-      </c>
-      <c r="M6" s="6" t="b">
-        <v>0</v>
-      </c>
-      <c r="N6" s="6" t="b">
-        <v>0</v>
-      </c>
-      <c r="O6" s="6" t="b">
-        <v>0</v>
-      </c>
-      <c r="P6" s="6" t="b">
-        <v>0</v>
-      </c>
-      <c r="Q6" s="6" t="b">
-        <v>0</v>
-      </c>
-      <c r="R6" s="6" t="b">
-        <v>0</v>
-      </c>
-      <c r="S6" s="6" t="b">
-        <v>0</v>
-      </c>
-      <c r="T6" s="6" t="b">
-        <v>0</v>
-      </c>
-      <c r="U6" s="6" t="b">
+      <c r="B6" s="9" t="b">
+        <v>0</v>
+      </c>
+      <c r="C6" s="9" t="b">
+        <v>0</v>
+      </c>
+      <c r="D6" s="9" t="b">
+        <v>0</v>
+      </c>
+      <c r="E6" s="9" t="b">
+        <v>0</v>
+      </c>
+      <c r="F6" s="9" t="b">
+        <v>0</v>
+      </c>
+      <c r="G6" s="9" t="b">
+        <v>0</v>
+      </c>
+      <c r="H6" s="9" t="b">
+        <v>0</v>
+      </c>
+      <c r="I6" s="9" t="b">
+        <v>0</v>
+      </c>
+      <c r="J6" s="9" t="b">
+        <v>0</v>
+      </c>
+      <c r="K6" s="9" t="b">
+        <v>0</v>
+      </c>
+      <c r="L6" s="9" t="b">
+        <v>0</v>
+      </c>
+      <c r="M6" s="9" t="b">
+        <v>0</v>
+      </c>
+      <c r="N6" s="9" t="b">
+        <v>0</v>
+      </c>
+      <c r="O6" s="9" t="b">
+        <v>0</v>
+      </c>
+      <c r="P6" s="9" t="b">
+        <v>0</v>
+      </c>
+      <c r="Q6" s="9" t="b">
+        <v>0</v>
+      </c>
+      <c r="R6" s="9" t="b">
+        <v>0</v>
+      </c>
+      <c r="S6" s="9" t="b">
+        <v>0</v>
+      </c>
+      <c r="T6" s="9" t="b">
+        <v>0</v>
+      </c>
+      <c r="U6" s="9" t="b">
         <v>0</v>
       </c>
     </row>
-    <row r="7" s="2" customFormat="1" spans="1:21">
-      <c r="A7" s="6" t="s">
+    <row r="7" s="3" customFormat="1" ht="14.25" spans="1:21">
+      <c r="A7" s="10" t="s">
         <v>28</v>
       </c>
-      <c r="B7" s="7"/>
-      <c r="C7" s="7"/>
-      <c r="D7" s="7"/>
-      <c r="E7" s="7"/>
-      <c r="F7" s="7"/>
-      <c r="G7" s="7"/>
-      <c r="H7" s="7"/>
-      <c r="I7" s="7"/>
-      <c r="J7" s="7"/>
-      <c r="K7" s="7"/>
-      <c r="L7" s="7"/>
-      <c r="M7" s="7"/>
-      <c r="N7" s="7"/>
-      <c r="O7" s="7"/>
-      <c r="P7" s="7"/>
-      <c r="Q7" s="6"/>
-      <c r="R7" s="6"/>
-      <c r="S7" s="6"/>
-      <c r="T7" s="6"/>
-      <c r="U7" s="6"/>
+      <c r="B7" s="11"/>
+      <c r="C7" s="11"/>
+      <c r="D7" s="11"/>
+      <c r="E7" s="11"/>
+      <c r="F7" s="11"/>
+      <c r="G7" s="11"/>
+      <c r="H7" s="11"/>
+      <c r="I7" s="11"/>
+      <c r="J7" s="11"/>
+      <c r="K7" s="11"/>
+      <c r="L7" s="11"/>
+      <c r="M7" s="11"/>
+      <c r="N7" s="11"/>
+      <c r="O7" s="11"/>
+      <c r="P7" s="11"/>
+      <c r="Q7" s="12"/>
+      <c r="R7" s="12"/>
+      <c r="S7" s="12"/>
+      <c r="T7" s="12"/>
+      <c r="U7" s="12"/>
     </row>
     <row r="8" spans="1:19">
       <c r="A8" t="s">

</xml_diff>